<commit_message>
Added 4 reward values in the loop
</commit_message>
<xml_diff>
--- a/Foraging task/Foraging task (Env 1)/reward1.xlsx
+++ b/Foraging task/Foraging task (Env 1)/reward1.xlsx
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t xml:space="preserve">rewardval</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rewardpos</t>
   </si>
 </sst>
 </file>
@@ -133,18 +130,16 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -157,9 +152,7 @@
       <c r="A2" s="0" t="n">
         <v>7.5</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>-0.2</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -169,9 +162,7 @@
       <c r="A3" s="0" t="n">
         <v>7.1</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>0.2</v>
-      </c>
+      <c r="B3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -181,9 +172,7 @@
       <c r="A4" s="0" t="n">
         <v>6.2</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>-0.2</v>
-      </c>
+      <c r="B4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -193,9 +182,7 @@
       <c r="A5" s="2" t="n">
         <v>5.9</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>0.2</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="2"/>
@@ -206,9 +193,7 @@
       <c r="A6" s="0" t="n">
         <v>5.1</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>-0.2</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -218,9 +203,7 @@
       <c r="A7" s="0" t="n">
         <v>4.8</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <v>0.2</v>
-      </c>
+      <c r="B7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="2"/>
       <c r="F7" s="1"/>
@@ -230,9 +213,7 @@
       <c r="A8" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="1" t="n">
-        <v>-0.2</v>
-      </c>
+      <c r="B8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -242,9 +223,7 @@
       <c r="A9" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="B9" s="1" t="n">
-        <v>0.2</v>
-      </c>
+      <c r="B9" s="1"/>
       <c r="D9" s="2"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -254,9 +233,7 @@
       <c r="A10" s="0" t="n">
         <v>2.6</v>
       </c>
-      <c r="B10" s="1" t="n">
-        <v>-0.2</v>
-      </c>
+      <c r="B10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -266,9 +243,7 @@
       <c r="A11" s="0" t="n">
         <v>2.1</v>
       </c>
-      <c r="B11" s="1" t="n">
-        <v>0.2</v>
-      </c>
+      <c r="B11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -278,9 +253,7 @@
       <c r="A12" s="0" t="n">
         <v>1.3</v>
       </c>
-      <c r="B12" s="1" t="n">
-        <v>-0.2</v>
-      </c>
+      <c r="B12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -290,9 +263,7 @@
       <c r="A13" s="0" t="n">
         <v>0.7</v>
       </c>
-      <c r="B13" s="1" t="n">
-        <v>0.2</v>
-      </c>
+      <c r="B13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -301,9 +272,6 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>0</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>-0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>